<commit_message>
Agrego complemento, en el commit anterior no se adjunto
</commit_message>
<xml_diff>
--- a/Base de datos Proveedores.xlsx
+++ b/Base de datos Proveedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Forero\Desktop\pago-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892A8364-C8E8-4797-9A98-521205057D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD985A6-96D6-4266-891A-188696EF838E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1815" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="151">
   <si>
     <t>Tipo de Identificacion</t>
   </si>
@@ -491,105 +491,6 @@
   </si>
   <si>
     <t>ALQUILER Y ALIMENTACIÓN</t>
-  </si>
-  <si>
-    <t>BIBO</t>
-  </si>
-  <si>
-    <t>SOLUTIONS SAS</t>
-  </si>
-  <si>
-    <t>CIMAZ</t>
-  </si>
-  <si>
-    <t>S.A.S</t>
-  </si>
-  <si>
-    <t>CIMPRE</t>
-  </si>
-  <si>
-    <t>SALUD OCUPACIONAL S.A.S.</t>
-  </si>
-  <si>
-    <t>DIANA</t>
-  </si>
-  <si>
-    <t>CARINA IMPATA RESTREPO</t>
-  </si>
-  <si>
-    <t>DIGITALTIC</t>
-  </si>
-  <si>
-    <t>DOMINGO</t>
-  </si>
-  <si>
-    <t>IGNACIO ROJAS</t>
-  </si>
-  <si>
-    <t>ELECTRICOS</t>
-  </si>
-  <si>
-    <t>DEL VALLE SA</t>
-  </si>
-  <si>
-    <t>ELECTRO</t>
-  </si>
-  <si>
-    <t>JAPONESA S.A.</t>
-  </si>
-  <si>
-    <t>GVS</t>
-  </si>
-  <si>
-    <t>COLOMBIA SAS</t>
-  </si>
-  <si>
-    <t>Hp</t>
-  </si>
-  <si>
-    <t>Financial Services Colombia LLC Sucursal Colombia</t>
-  </si>
-  <si>
-    <t>IZC</t>
-  </si>
-  <si>
-    <t>MAYORISTA SAS</t>
-  </si>
-  <si>
-    <t>JUAN</t>
-  </si>
-  <si>
-    <t>CARLOS MARQUEZ 	SANCHEZ</t>
-  </si>
-  <si>
-    <t>LILIUM</t>
-  </si>
-  <si>
-    <t>TECNOLOGIA SAS</t>
-  </si>
-  <si>
-    <t>NEXSYS</t>
-  </si>
-  <si>
-    <t>DE COLOMBIA SA</t>
-  </si>
-  <si>
-    <t>RENTEK</t>
-  </si>
-  <si>
-    <t>TIENDAS</t>
-  </si>
-  <si>
-    <t>TECNOPLAZA S.A.S</t>
-  </si>
-  <si>
-    <t>WILLIAM</t>
-  </si>
-  <si>
-    <t>ROJAS SALAZAR</t>
-  </si>
-  <si>
-    <t>YAMAKI</t>
   </si>
 </sst>
 </file>
@@ -1175,12 +1076,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,474 +1128,6 @@
       </c>
       <c r="J1" s="46" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="44">
-        <v>1</v>
-      </c>
-      <c r="B2" s="45">
-        <v>900858550</v>
-      </c>
-      <c r="C2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="44">
-        <v>5</v>
-      </c>
-      <c r="F2" s="44">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6">
-        <v>2359386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="44">
-        <v>1</v>
-      </c>
-      <c r="B3" s="45">
-        <v>900654100</v>
-      </c>
-      <c r="C3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" s="44">
-        <v>4554</v>
-      </c>
-      <c r="F3" s="44">
-        <v>65456</v>
-      </c>
-      <c r="G3">
-        <v>56456</v>
-      </c>
-      <c r="H3" s="6">
-        <v>525870</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
-        <v>1</v>
-      </c>
-      <c r="B4" s="45">
-        <v>1143940723</v>
-      </c>
-      <c r="C4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="44">
-        <v>64564</v>
-      </c>
-      <c r="F4" s="44">
-        <v>56456</v>
-      </c>
-      <c r="G4">
-        <v>456456</v>
-      </c>
-      <c r="H4" s="6">
-        <v>87451</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
-        <v>3</v>
-      </c>
-      <c r="B5" s="45">
-        <v>31322510</v>
-      </c>
-      <c r="C5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E5" s="44">
-        <v>456456</v>
-      </c>
-      <c r="F5" s="44">
-        <v>4564556</v>
-      </c>
-      <c r="G5">
-        <v>456456</v>
-      </c>
-      <c r="H5" s="6">
-        <v>84300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="44">
-        <v>1</v>
-      </c>
-      <c r="B6" s="45">
-        <v>901223156</v>
-      </c>
-      <c r="C6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="44">
-        <v>56456456</v>
-      </c>
-      <c r="F6" s="44">
-        <v>546456</v>
-      </c>
-      <c r="G6">
-        <v>456456</v>
-      </c>
-      <c r="H6" s="6">
-        <v>193970</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="44">
-        <v>3</v>
-      </c>
-      <c r="B7" s="45">
-        <v>7215649</v>
-      </c>
-      <c r="C7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="44">
-        <v>456456</v>
-      </c>
-      <c r="F7" s="44">
-        <v>45646</v>
-      </c>
-      <c r="G7">
-        <v>456456</v>
-      </c>
-      <c r="H7" s="6">
-        <v>97991</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="44">
-        <v>1</v>
-      </c>
-      <c r="B8" s="45">
-        <v>890304345</v>
-      </c>
-      <c r="C8" t="s">
-        <v>162</v>
-      </c>
-      <c r="D8" t="s">
-        <v>163</v>
-      </c>
-      <c r="E8" s="44">
-        <v>456456</v>
-      </c>
-      <c r="F8" s="44">
-        <v>456456</v>
-      </c>
-      <c r="G8">
-        <v>6456456</v>
-      </c>
-      <c r="H8" s="6">
-        <v>172500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="44">
-        <v>1</v>
-      </c>
-      <c r="B9" s="45">
-        <v>890306372</v>
-      </c>
-      <c r="C9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" s="44">
-        <v>56456</v>
-      </c>
-      <c r="F9" s="44">
-        <v>456456</v>
-      </c>
-      <c r="G9">
-        <v>56456</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1819546</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="44">
-        <v>1</v>
-      </c>
-      <c r="B10" s="45">
-        <v>900298074</v>
-      </c>
-      <c r="C10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D10" t="s">
-        <v>167</v>
-      </c>
-      <c r="E10" s="44">
-        <v>56456</v>
-      </c>
-      <c r="F10" s="44">
-        <v>456456</v>
-      </c>
-      <c r="G10">
-        <v>456456</v>
-      </c>
-      <c r="H10" s="6">
-        <v>9952604</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="44">
-        <v>1</v>
-      </c>
-      <c r="B11" s="45">
-        <v>830076882</v>
-      </c>
-      <c r="C11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D11" t="s">
-        <v>169</v>
-      </c>
-      <c r="E11" s="44">
-        <v>56456</v>
-      </c>
-      <c r="F11" s="44">
-        <v>564564</v>
-      </c>
-      <c r="G11">
-        <v>45645645</v>
-      </c>
-      <c r="H11" s="6">
-        <v>4407849</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="44">
-        <v>1</v>
-      </c>
-      <c r="B12" s="45">
-        <v>1143940722</v>
-      </c>
-      <c r="C12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D12" t="s">
-        <v>171</v>
-      </c>
-      <c r="E12" s="44">
-        <v>5645645</v>
-      </c>
-      <c r="F12" s="44">
-        <v>456456</v>
-      </c>
-      <c r="G12">
-        <v>4564565</v>
-      </c>
-      <c r="H12" s="6">
-        <v>52092009</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="44">
-        <v>1</v>
-      </c>
-      <c r="B13" s="45">
-        <v>94281756</v>
-      </c>
-      <c r="C13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D13" t="s">
-        <v>173</v>
-      </c>
-      <c r="E13" s="44">
-        <v>56456</v>
-      </c>
-      <c r="F13" s="44">
-        <v>456456</v>
-      </c>
-      <c r="G13">
-        <v>45645645</v>
-      </c>
-      <c r="H13" s="6">
-        <v>1074121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
-        <v>1</v>
-      </c>
-      <c r="B14" s="45">
-        <v>900892841</v>
-      </c>
-      <c r="C14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D14" t="s">
-        <v>175</v>
-      </c>
-      <c r="E14" s="44">
-        <v>54645645</v>
-      </c>
-      <c r="F14" s="44">
-        <v>456456456</v>
-      </c>
-      <c r="G14">
-        <v>456456</v>
-      </c>
-      <c r="H14" s="6">
-        <v>669600</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="44">
-        <v>1</v>
-      </c>
-      <c r="B15" s="45">
-        <v>800035776</v>
-      </c>
-      <c r="C15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D15" t="s">
-        <v>177</v>
-      </c>
-      <c r="E15" s="44">
-        <v>45645645</v>
-      </c>
-      <c r="F15" s="44">
-        <v>546456</v>
-      </c>
-      <c r="G15">
-        <v>456456</v>
-      </c>
-      <c r="H15" s="6">
-        <v>18089916</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
-        <v>1</v>
-      </c>
-      <c r="B16" s="45">
-        <v>830034343</v>
-      </c>
-      <c r="C16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="44">
-        <v>56456</v>
-      </c>
-      <c r="F16" s="44">
-        <v>456456</v>
-      </c>
-      <c r="G16">
-        <v>456456</v>
-      </c>
-      <c r="H16" s="6">
-        <v>4094318</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="44">
-        <v>1</v>
-      </c>
-      <c r="B17" s="45">
-        <v>900355222</v>
-      </c>
-      <c r="C17" t="s">
-        <v>179</v>
-      </c>
-      <c r="D17" t="s">
-        <v>180</v>
-      </c>
-      <c r="E17" s="44">
-        <v>45645656</v>
-      </c>
-      <c r="F17" s="44">
-        <v>546456</v>
-      </c>
-      <c r="G17">
-        <v>456456</v>
-      </c>
-      <c r="H17" s="6">
-        <v>492503</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
-        <v>3</v>
-      </c>
-      <c r="B18" s="45">
-        <v>7685100</v>
-      </c>
-      <c r="C18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D18" t="s">
-        <v>182</v>
-      </c>
-      <c r="E18" s="44">
-        <v>456456</v>
-      </c>
-      <c r="F18" s="44">
-        <v>456456</v>
-      </c>
-      <c r="G18">
-        <v>456456456</v>
-      </c>
-      <c r="H18" s="6">
-        <v>6013778</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="44">
-        <v>1</v>
-      </c>
-      <c r="B19" s="45">
-        <v>800179308</v>
-      </c>
-      <c r="C19" t="s">
-        <v>183</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="44">
-        <v>456456</v>
-      </c>
-      <c r="F19" s="44">
-        <v>456456</v>
-      </c>
-      <c r="G19">
-        <v>456456</v>
-      </c>
-      <c r="H19" s="6">
-        <v>4031339</v>
       </c>
     </row>
   </sheetData>
@@ -2992,9 +2425,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3221,27 +2657,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
-    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3266,9 +2690,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
+    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
en el formulario se agrega nombre del banco al que pertenece el numero de identificacion
</commit_message>
<xml_diff>
--- a/Base de datos Proveedores.xlsx
+++ b/Base de datos Proveedores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Forero\Desktop\pago-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD985A6-96D6-4266-891A-188696EF838E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C40BE97-8B89-40AD-B267-DA32BA324B94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1815" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1081,7 +1081,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,8 +1131,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J4111">
-    <sortCondition ref="B2:B4111"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J4086">
+    <sortCondition ref="B2:B4086"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2434,6 +2434,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002B6B606D19F8C64C9C79835747E2E002" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1490ca6afe76db67316394b374b3fffa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a52c2c93-1616-4696-bc88-4a2586572708" xmlns:ns4="44ef142f-35ce-48df-bc44-191ee5827fd0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f03ce17d5f7f795edd6d7d0ee76cdef5" ns3:_="" ns4:_="">
     <xsd:import namespace="a52c2c93-1616-4696-bc88-4a2586572708"/>
@@ -2656,12 +2662,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
   <ds:schemaRefs>
@@ -2671,6 +2671,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
+    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E61E25-AEDA-4F7D-AB2D-2A0978BE05A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2687,21 +2704,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="44ef142f-35ce-48df-bc44-191ee5827fd0"/>
-    <ds:schemaRef ds:uri="a52c2c93-1616-4696-bc88-4a2586572708"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
se agrega el boton del formulario cancelar; cancela toda la macro
</commit_message>
<xml_diff>
--- a/Base de datos Proveedores.xlsx
+++ b/Base de datos Proveedores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Forero\Desktop\pago-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C40BE97-8B89-40AD-B267-DA32BA324B94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4391C2D-AB0C-4818-8267-F0105DC36D79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1815" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
   <si>
     <t>Tipo de Identificacion</t>
   </si>
@@ -491,6 +491,39 @@
   </si>
   <si>
     <t>ALQUILER Y ALIMENTACIÓN</t>
+  </si>
+  <si>
+    <t>BIBO</t>
+  </si>
+  <si>
+    <t>SOLUTIONS SAS</t>
+  </si>
+  <si>
+    <t>CIMAZ</t>
+  </si>
+  <si>
+    <t>S.A.S</t>
+  </si>
+  <si>
+    <t>CIMPRE</t>
+  </si>
+  <si>
+    <t>SALUD OCUPACIONAL S.A.S.</t>
+  </si>
+  <si>
+    <t>DIANA</t>
+  </si>
+  <si>
+    <t>CARINA IMPATA RESTREPO</t>
+  </si>
+  <si>
+    <t>DIGITALTIC</t>
+  </si>
+  <si>
+    <t>DOMINGO</t>
+  </si>
+  <si>
+    <t>IGNACIO ROJAS</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1109,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1128,6 +1161,162 @@
       </c>
       <c r="J1" s="46" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="44">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45">
+        <v>900858550</v>
+      </c>
+      <c r="C2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="44">
+        <v>7</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>6456465</v>
+      </c>
+      <c r="H2" s="6">
+        <v>2359386</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="44">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45">
+        <v>900654100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="44">
+        <v>7</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>654546</v>
+      </c>
+      <c r="H3" s="6">
+        <v>525870</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="44">
+        <v>1</v>
+      </c>
+      <c r="B4" s="45">
+        <v>1143940723</v>
+      </c>
+      <c r="C4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="44">
+        <v>7</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>5646545</v>
+      </c>
+      <c r="H4" s="6">
+        <v>87451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>3</v>
+      </c>
+      <c r="B5" s="45">
+        <v>31322510</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="44">
+        <v>1051</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>654654</v>
+      </c>
+      <c r="H5" s="6">
+        <v>84300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="44">
+        <v>1</v>
+      </c>
+      <c r="B6" s="45">
+        <v>901223156</v>
+      </c>
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="44">
+        <v>1057</v>
+      </c>
+      <c r="F6" s="44">
+        <v>46546</v>
+      </c>
+      <c r="G6">
+        <v>645654</v>
+      </c>
+      <c r="H6" s="6">
+        <v>193970</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="44">
+        <v>3</v>
+      </c>
+      <c r="B7" s="45">
+        <v>7215649</v>
+      </c>
+      <c r="C7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="44">
+        <v>1057</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>64654</v>
+      </c>
+      <c r="H7" s="6">
+        <v>97991</v>
       </c>
     </row>
   </sheetData>
@@ -2425,21 +2614,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002B6B606D19F8C64C9C79835747E2E002" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1490ca6afe76db67316394b374b3fffa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a52c2c93-1616-4696-bc88-4a2586572708" xmlns:ns4="44ef142f-35ce-48df-bc44-191ee5827fd0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f03ce17d5f7f795edd6d7d0ee76cdef5" ns3:_="" ns4:_="">
     <xsd:import namespace="a52c2c93-1616-4696-bc88-4a2586572708"/>
@@ -2662,15 +2842,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEA6490E-A2D4-4F41-902E-623575711A1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2687,7 +2868,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E61E25-AEDA-4F7D-AB2D-2A0978BE05A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2704,4 +2885,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4CA132-BAA9-487C-B8CA-1DC25345625A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>